<commit_message>
Update automatico via Actualizar 05-21-2020 19-24-19
</commit_message>
<xml_diff>
--- a/datacovidgt/00 DATACOVID_GT_CUARENTENA.xlsx
+++ b/datacovidgt/00 DATACOVID_GT_CUARENTENA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22918"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/CORONA VIRUS/DATACOVID GT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="152" documentId="8_{A9F190C0-AECD-4B67-9C8B-6A53EABFC553}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F4B85275-2FF2-4488-98D6-30D7C0533B08}"/>
+  <xr:revisionPtr revIDLastSave="160" documentId="8_{A9F190C0-AECD-4B67-9C8B-6A53EABFC553}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2A34048A-F894-4BFD-B9EA-713D5C539B4F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1063" uniqueCount="373">
   <si>
     <t>Id_Dep</t>
   </si>
@@ -687,6 +687,12 @@
   </si>
   <si>
     <t>Malacatán</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>No se permite el ingreso y egreso de personas al municipio por ser foco de contagio en dicho lugar se reportan 33 casos positivos y de ahi se ha extendido a otros municipios del Departamento de San Marcos</t>
   </si>
   <si>
     <t>Catarina</t>
@@ -1831,12 +1837,12 @@
   <autoFilter ref="A10:K351" xr:uid="{7D8986B2-82D7-4C79-8B4E-BA728CF7C5D1}">
     <filterColumn colId="2">
       <filters>
-        <filter val="Almolonga"/>
+        <filter val="Malacatán"/>
       </filters>
     </filterColumn>
     <filterColumn colId="3">
       <filters>
-        <filter val="Guatemala"/>
+        <filter val="San Marcos"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -2157,8 +2163,8 @@
   <dimension ref="A10:K351"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10:I10"/>
+      <pane ySplit="10" topLeftCell="A352" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K355" sqref="K355"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
@@ -7136,7 +7142,7 @@
       <c r="J191" s="8"/>
       <c r="K191" s="9"/>
     </row>
-    <row r="192" spans="1:11" ht="15.6" hidden="1">
+    <row r="192" spans="1:11" ht="67.5">
       <c r="A192" s="2">
         <v>12</v>
       </c>
@@ -7158,10 +7164,16 @@
       <c r="G192" s="3">
         <v>14.9344199816</v>
       </c>
-      <c r="H192" s="8"/>
+      <c r="H192" s="8" t="s">
+        <v>212</v>
+      </c>
       <c r="I192" s="9"/>
-      <c r="J192" s="8"/>
-      <c r="K192" s="9"/>
+      <c r="J192" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="K192" s="9" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="193" spans="1:11" ht="15.6" hidden="1">
       <c r="A193" s="2">
@@ -7171,7 +7183,7 @@
         <v>1216</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="D193" s="1" t="s">
         <v>198</v>
@@ -7198,7 +7210,7 @@
         <v>1217</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D194" s="1" t="s">
         <v>198</v>
@@ -7225,7 +7237,7 @@
         <v>1218</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="D195" s="1" t="s">
         <v>198</v>
@@ -7252,7 +7264,7 @@
         <v>1219</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D196" s="1" t="s">
         <v>198</v>
@@ -7279,7 +7291,7 @@
         <v>1220</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D197" s="1" t="s">
         <v>198</v>
@@ -7306,7 +7318,7 @@
         <v>1221</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D198" s="1" t="s">
         <v>198</v>
@@ -7333,7 +7345,7 @@
         <v>1222</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="D199" s="1" t="s">
         <v>198</v>
@@ -7360,7 +7372,7 @@
         <v>1223</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D200" s="1" t="s">
         <v>198</v>
@@ -7387,7 +7399,7 @@
         <v>1224</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D201" s="1" t="s">
         <v>198</v>
@@ -7414,7 +7426,7 @@
         <v>1225</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="D202" s="1" t="s">
         <v>198</v>
@@ -7441,7 +7453,7 @@
         <v>1226</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="D203" s="1" t="s">
         <v>198</v>
@@ -7468,7 +7480,7 @@
         <v>1227</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="D204" s="1" t="s">
         <v>198</v>
@@ -7495,7 +7507,7 @@
         <v>1228</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="D205" s="1" t="s">
         <v>198</v>
@@ -7549,7 +7561,7 @@
         <v>1230</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D207" s="1" t="s">
         <v>198</v>
@@ -7576,10 +7588,10 @@
         <v>1301</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E208" t="s">
         <v>129</v>
@@ -7603,10 +7615,10 @@
         <v>1302</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E209" t="s">
         <v>129</v>
@@ -7630,10 +7642,10 @@
         <v>1303</v>
       </c>
       <c r="C210" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D210" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="D210" s="1" t="s">
-        <v>226</v>
       </c>
       <c r="E210" t="s">
         <v>129</v>
@@ -7657,10 +7669,10 @@
         <v>1304</v>
       </c>
       <c r="C211" s="1" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E211" t="s">
         <v>129</v>
@@ -7684,10 +7696,10 @@
         <v>1305</v>
       </c>
       <c r="C212" s="1" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E212" t="s">
         <v>129</v>
@@ -7711,10 +7723,10 @@
         <v>1306</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E213" t="s">
         <v>129</v>
@@ -7738,10 +7750,10 @@
         <v>1307</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E214" t="s">
         <v>129</v>
@@ -7765,10 +7777,10 @@
         <v>1308</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E215" t="s">
         <v>129</v>
@@ -7796,10 +7808,10 @@
         <v>1309</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E216" t="s">
         <v>129</v>
@@ -7826,7 +7838,7 @@
         <v>182</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E217" t="s">
         <v>129</v>
@@ -7850,10 +7862,10 @@
         <v>1311</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E218" t="s">
         <v>129</v>
@@ -7880,7 +7892,7 @@
         <v>80</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E219" t="s">
         <v>129</v>
@@ -7904,10 +7916,10 @@
         <v>1313</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D220" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E220" t="s">
         <v>129</v>
@@ -7931,10 +7943,10 @@
         <v>1314</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E221" t="s">
         <v>129</v>
@@ -7958,10 +7970,10 @@
         <v>1315</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E222" t="s">
         <v>129</v>
@@ -7985,10 +7997,10 @@
         <v>1316</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E223" t="s">
         <v>129</v>
@@ -8012,10 +8024,10 @@
         <v>1317</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E224" t="s">
         <v>129</v>
@@ -8039,10 +8051,10 @@
         <v>1318</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="D225" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E225" t="s">
         <v>129</v>
@@ -8066,10 +8078,10 @@
         <v>1319</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E226" t="s">
         <v>129</v>
@@ -8093,10 +8105,10 @@
         <v>1320</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="D227" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E227" t="s">
         <v>129</v>
@@ -8120,10 +8132,10 @@
         <v>1321</v>
       </c>
       <c r="C228" s="1" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E228" t="s">
         <v>129</v>
@@ -8147,10 +8159,10 @@
         <v>1322</v>
       </c>
       <c r="C229" s="1" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="D229" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E229" t="s">
         <v>129</v>
@@ -8174,10 +8186,10 @@
         <v>1323</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E230" t="s">
         <v>129</v>
@@ -8201,10 +8213,10 @@
         <v>1324</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="D231" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E231" t="s">
         <v>129</v>
@@ -8228,10 +8240,10 @@
         <v>1325</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="D232" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E232" t="s">
         <v>129</v>
@@ -8255,10 +8267,10 @@
         <v>1326</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="D233" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E233" t="s">
         <v>129</v>
@@ -8282,10 +8294,10 @@
         <v>1327</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="D234" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E234" t="s">
         <v>129</v>
@@ -8309,10 +8321,10 @@
         <v>1328</v>
       </c>
       <c r="C235" s="1" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="D235" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E235" t="s">
         <v>129</v>
@@ -8336,10 +8348,10 @@
         <v>1329</v>
       </c>
       <c r="C236" s="1" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="D236" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E236" t="s">
         <v>129</v>
@@ -8363,10 +8375,10 @@
         <v>1330</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="D237" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E237" t="s">
         <v>129</v>
@@ -8390,10 +8402,10 @@
         <v>1331</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="D238" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E238" t="s">
         <v>129</v>
@@ -8417,10 +8429,10 @@
         <v>1332</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D239" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E239" t="s">
         <v>129</v>
@@ -8444,10 +8456,10 @@
         <v>1333</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="D240" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E240" t="s">
         <v>129</v>
@@ -8471,10 +8483,10 @@
         <v>1401</v>
       </c>
       <c r="C241" s="1" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="D241" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E241" t="s">
         <v>109</v>
@@ -8498,10 +8510,10 @@
         <v>1402</v>
       </c>
       <c r="C242" s="1" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="D242" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E242" t="s">
         <v>109</v>
@@ -8525,10 +8537,10 @@
         <v>1403</v>
       </c>
       <c r="C243" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D243" s="1" t="s">
         <v>260</v>
-      </c>
-      <c r="D243" s="1" t="s">
-        <v>258</v>
       </c>
       <c r="E243" t="s">
         <v>109</v>
@@ -8552,10 +8564,10 @@
         <v>1404</v>
       </c>
       <c r="C244" s="1" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D244" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E244" t="s">
         <v>109</v>
@@ -8579,10 +8591,10 @@
         <v>1405</v>
       </c>
       <c r="C245" s="1" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="D245" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E245" t="s">
         <v>109</v>
@@ -8606,10 +8618,10 @@
         <v>1406</v>
       </c>
       <c r="C246" s="1" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="D246" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E246" t="s">
         <v>109</v>
@@ -8633,10 +8645,10 @@
         <v>1407</v>
       </c>
       <c r="C247" s="1" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="D247" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E247" t="s">
         <v>109</v>
@@ -8660,10 +8672,10 @@
         <v>1408</v>
       </c>
       <c r="C248" s="1" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="D248" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E248" t="s">
         <v>109</v>
@@ -8687,10 +8699,10 @@
         <v>1409</v>
       </c>
       <c r="C249" s="1" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="D249" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E249" t="s">
         <v>109</v>
@@ -8714,10 +8726,10 @@
         <v>1410</v>
       </c>
       <c r="C250" s="1" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="D250" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E250" t="s">
         <v>109</v>
@@ -8741,10 +8753,10 @@
         <v>1411</v>
       </c>
       <c r="C251" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D251" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E251" t="s">
         <v>109</v>
@@ -8768,10 +8780,10 @@
         <v>1412</v>
       </c>
       <c r="C252" s="1" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="D252" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E252" t="s">
         <v>109</v>
@@ -8795,10 +8807,10 @@
         <v>1413</v>
       </c>
       <c r="C253" s="1" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="D253" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E253" t="s">
         <v>109</v>
@@ -8822,10 +8834,10 @@
         <v>1414</v>
       </c>
       <c r="C254" s="1" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="D254" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E254" t="s">
         <v>109</v>
@@ -8849,10 +8861,10 @@
         <v>1415</v>
       </c>
       <c r="C255" s="1" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="D255" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E255" t="s">
         <v>109</v>
@@ -8876,10 +8888,10 @@
         <v>1416</v>
       </c>
       <c r="C256" s="1" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="D256" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E256" t="s">
         <v>109</v>
@@ -8903,10 +8915,10 @@
         <v>1417</v>
       </c>
       <c r="C257" s="1" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="D257" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E257" t="s">
         <v>109</v>
@@ -8930,10 +8942,10 @@
         <v>1418</v>
       </c>
       <c r="C258" s="1" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="D258" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E258" t="s">
         <v>109</v>
@@ -8957,10 +8969,10 @@
         <v>1419</v>
       </c>
       <c r="C259" s="1" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="D259" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E259" t="s">
         <v>109</v>
@@ -8984,10 +8996,10 @@
         <v>1420</v>
       </c>
       <c r="C260" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D260" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E260" t="s">
         <v>109</v>
@@ -9011,10 +9023,10 @@
         <v>1421</v>
       </c>
       <c r="C261" s="1" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="D261" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E261" t="s">
         <v>109</v>
@@ -9038,10 +9050,10 @@
         <v>1501</v>
       </c>
       <c r="C262" s="1" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="D262" s="1" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E262" t="s">
         <v>109</v>
@@ -9065,10 +9077,10 @@
         <v>1502</v>
       </c>
       <c r="C263" s="1" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="D263" s="1" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E263" t="s">
         <v>109</v>
@@ -9092,10 +9104,10 @@
         <v>1503</v>
       </c>
       <c r="C264" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="D264" s="1" t="s">
         <v>282</v>
-      </c>
-      <c r="D264" s="1" t="s">
-        <v>280</v>
       </c>
       <c r="E264" t="s">
         <v>109</v>
@@ -9119,10 +9131,10 @@
         <v>1504</v>
       </c>
       <c r="C265" s="1" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="D265" s="1" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E265" t="s">
         <v>109</v>
@@ -9146,10 +9158,10 @@
         <v>1505</v>
       </c>
       <c r="C266" s="1" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="D266" s="1" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E266" t="s">
         <v>109</v>
@@ -9173,10 +9185,10 @@
         <v>1506</v>
       </c>
       <c r="C267" s="1" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="D267" s="1" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E267" t="s">
         <v>109</v>
@@ -9200,10 +9212,10 @@
         <v>1507</v>
       </c>
       <c r="C268" s="1" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="D268" s="1" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E268" t="s">
         <v>109</v>
@@ -9227,10 +9239,10 @@
         <v>1508</v>
       </c>
       <c r="C269" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="D269" s="1" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E269" t="s">
         <v>109</v>
@@ -9254,10 +9266,10 @@
         <v>1601</v>
       </c>
       <c r="C270" s="1" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="D270" s="1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="E270" t="s">
         <v>109</v>
@@ -9281,10 +9293,10 @@
         <v>1602</v>
       </c>
       <c r="C271" s="1" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="D271" s="1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="E271" t="s">
         <v>109</v>
@@ -9308,10 +9320,10 @@
         <v>1603</v>
       </c>
       <c r="C272" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="D272" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="D272" s="1" t="s">
-        <v>289</v>
       </c>
       <c r="E272" t="s">
         <v>109</v>
@@ -9335,10 +9347,10 @@
         <v>1604</v>
       </c>
       <c r="C273" s="1" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="D273" s="1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="E273" t="s">
         <v>109</v>
@@ -9362,10 +9374,10 @@
         <v>1605</v>
       </c>
       <c r="C274" s="1" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="D274" s="1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="E274" t="s">
         <v>109</v>
@@ -9389,10 +9401,10 @@
         <v>1606</v>
       </c>
       <c r="C275" s="1" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="D275" s="1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="E275" t="s">
         <v>109</v>
@@ -9416,10 +9428,10 @@
         <v>1607</v>
       </c>
       <c r="C276" s="1" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="D276" s="1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="E276" t="s">
         <v>109</v>
@@ -9443,10 +9455,10 @@
         <v>1608</v>
       </c>
       <c r="C277" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="D277" s="1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="E277" t="s">
         <v>109</v>
@@ -9470,10 +9482,10 @@
         <v>1609</v>
       </c>
       <c r="C278" s="1" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="D278" s="1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="E278" t="s">
         <v>109</v>
@@ -9497,10 +9509,10 @@
         <v>1610</v>
       </c>
       <c r="C279" s="1" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="D279" s="1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="E279" t="s">
         <v>109</v>
@@ -9524,10 +9536,10 @@
         <v>1611</v>
       </c>
       <c r="C280" s="1" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="D280" s="1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="E280" t="s">
         <v>109</v>
@@ -9551,10 +9563,10 @@
         <v>1612</v>
       </c>
       <c r="C281" s="1" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="D281" s="1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="E281" t="s">
         <v>109</v>
@@ -9578,10 +9590,10 @@
         <v>1613</v>
       </c>
       <c r="C282" s="1" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="D282" s="1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="E282" t="s">
         <v>109</v>
@@ -9605,10 +9617,10 @@
         <v>1614</v>
       </c>
       <c r="C283" s="1" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="D283" s="1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="E283" t="s">
         <v>109</v>
@@ -9632,10 +9644,10 @@
         <v>1615</v>
       </c>
       <c r="C284" s="1" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="D284" s="1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="E284" t="s">
         <v>109</v>
@@ -9659,10 +9671,10 @@
         <v>1616</v>
       </c>
       <c r="C285" s="1" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="D285" s="1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="E285" t="s">
         <v>109</v>
@@ -9686,10 +9698,10 @@
         <v>1617</v>
       </c>
       <c r="C286" s="1" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="D286" s="1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="E286" t="s">
         <v>109</v>
@@ -9713,10 +9725,10 @@
         <v>1701</v>
       </c>
       <c r="C287" s="1" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="D287" s="1" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="E287" t="s">
         <v>109</v>
@@ -9743,7 +9755,7 @@
         <v>86</v>
       </c>
       <c r="D288" s="1" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="E288" t="s">
         <v>109</v>
@@ -9767,10 +9779,10 @@
         <v>1703</v>
       </c>
       <c r="C289" s="1" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="D289" s="1" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="E289" t="s">
         <v>109</v>
@@ -9794,10 +9806,10 @@
         <v>1704</v>
       </c>
       <c r="C290" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="D290" s="1" t="s">
         <v>309</v>
-      </c>
-      <c r="D290" s="1" t="s">
-        <v>307</v>
       </c>
       <c r="E290" t="s">
         <v>109</v>
@@ -9821,10 +9833,10 @@
         <v>1705</v>
       </c>
       <c r="C291" s="1" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="D291" s="1" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="E291" t="s">
         <v>109</v>
@@ -9848,10 +9860,10 @@
         <v>1706</v>
       </c>
       <c r="C292" s="1" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="D292" s="1" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="E292" t="s">
         <v>109</v>
@@ -9875,10 +9887,10 @@
         <v>1707</v>
       </c>
       <c r="C293" s="1" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="D293" s="1" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="E293" t="s">
         <v>109</v>
@@ -9902,10 +9914,10 @@
         <v>1708</v>
       </c>
       <c r="C294" s="1" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="D294" s="1" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="E294" t="s">
         <v>109</v>
@@ -9929,10 +9941,10 @@
         <v>1709</v>
       </c>
       <c r="C295" s="1" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="D295" s="1" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="E295" t="s">
         <v>109</v>
@@ -9956,10 +9968,10 @@
         <v>1710</v>
       </c>
       <c r="C296" s="1" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="D296" s="1" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="E296" t="s">
         <v>109</v>
@@ -9983,10 +9995,10 @@
         <v>1711</v>
       </c>
       <c r="C297" s="1" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="D297" s="1" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="E297" t="s">
         <v>109</v>
@@ -10010,10 +10022,10 @@
         <v>1712</v>
       </c>
       <c r="C298" s="1" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D298" s="1" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="E298" t="s">
         <v>109</v>
@@ -10037,10 +10049,10 @@
         <v>1713</v>
       </c>
       <c r="C299" s="1" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="D299" s="1" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="E299" t="s">
         <v>109</v>
@@ -10064,10 +10076,10 @@
         <v>1714</v>
       </c>
       <c r="C300" s="1" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D300" s="1" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="E300" t="s">
         <v>109</v>
@@ -10091,10 +10103,10 @@
         <v>1801</v>
       </c>
       <c r="C301" s="1" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="D301" s="1" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="E301" t="s">
         <v>33</v>
@@ -10118,10 +10130,10 @@
         <v>1802</v>
       </c>
       <c r="C302" s="1" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="D302" s="1" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="E302" t="s">
         <v>33</v>
@@ -10145,10 +10157,10 @@
         <v>1803</v>
       </c>
       <c r="C303" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D303" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="D303" s="1" t="s">
-        <v>320</v>
       </c>
       <c r="E303" t="s">
         <v>33</v>
@@ -10172,10 +10184,10 @@
         <v>1804</v>
       </c>
       <c r="C304" s="1" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="D304" s="1" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="E304" t="s">
         <v>33</v>
@@ -10199,10 +10211,10 @@
         <v>1805</v>
       </c>
       <c r="C305" s="1" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="D305" s="1" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="E305" t="s">
         <v>33</v>
@@ -10226,10 +10238,10 @@
         <v>1901</v>
       </c>
       <c r="C306" s="1" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="D306" s="1" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="E306" t="s">
         <v>33</v>
@@ -10253,10 +10265,10 @@
         <v>1902</v>
       </c>
       <c r="C307" s="1" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="D307" s="1" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="E307" t="s">
         <v>33</v>
@@ -10280,10 +10292,10 @@
         <v>1903</v>
       </c>
       <c r="C308" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="D308" s="1" t="s">
         <v>327</v>
-      </c>
-      <c r="D308" s="1" t="s">
-        <v>325</v>
       </c>
       <c r="E308" t="s">
         <v>33</v>
@@ -10307,10 +10319,10 @@
         <v>1904</v>
       </c>
       <c r="C309" s="1" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D309" s="1" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="E309" t="s">
         <v>33</v>
@@ -10325,7 +10337,7 @@
         <v>14</v>
       </c>
       <c r="I309" s="9" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="J309" s="8"/>
       <c r="K309" s="9"/>
@@ -10338,10 +10350,10 @@
         <v>1905</v>
       </c>
       <c r="C310" s="1" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="D310" s="1" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="E310" t="s">
         <v>33</v>
@@ -10356,7 +10368,7 @@
         <v>14</v>
       </c>
       <c r="I310" s="9" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="J310" s="8"/>
       <c r="K310" s="9"/>
@@ -10369,10 +10381,10 @@
         <v>1906</v>
       </c>
       <c r="C311" s="1" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="D311" s="1" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="E311" t="s">
         <v>33</v>
@@ -10396,10 +10408,10 @@
         <v>1907</v>
       </c>
       <c r="C312" s="1" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="D312" s="1" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="E312" t="s">
         <v>33</v>
@@ -10423,10 +10435,10 @@
         <v>1908</v>
       </c>
       <c r="C313" s="1" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D313" s="1" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="E313" t="s">
         <v>33</v>
@@ -10450,10 +10462,10 @@
         <v>1909</v>
       </c>
       <c r="C314" s="1" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D314" s="1" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="E314" t="s">
         <v>33</v>
@@ -10477,10 +10489,10 @@
         <v>1910</v>
       </c>
       <c r="C315" s="1" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D315" s="1" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="E315" t="s">
         <v>33</v>
@@ -10504,10 +10516,10 @@
         <v>1911</v>
       </c>
       <c r="C316" s="1" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="D316" s="1" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="E316" t="s">
         <v>33</v>
@@ -10531,10 +10543,10 @@
         <v>2001</v>
       </c>
       <c r="C317" s="1" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="D317" s="1" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="E317" t="s">
         <v>33</v>
@@ -10558,10 +10570,10 @@
         <v>2002</v>
       </c>
       <c r="C318" s="1" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="D318" s="1" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="E318" t="s">
         <v>33</v>
@@ -10585,10 +10597,10 @@
         <v>2003</v>
       </c>
       <c r="C319" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="D319" s="1" t="s">
         <v>339</v>
-      </c>
-      <c r="D319" s="1" t="s">
-        <v>337</v>
       </c>
       <c r="E319" t="s">
         <v>33</v>
@@ -10612,10 +10624,10 @@
         <v>2004</v>
       </c>
       <c r="C320" s="1" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="D320" s="1" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="E320" t="s">
         <v>33</v>
@@ -10639,10 +10651,10 @@
         <v>2005</v>
       </c>
       <c r="C321" s="1" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="D321" s="1" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="E321" t="s">
         <v>33</v>
@@ -10666,10 +10678,10 @@
         <v>2006</v>
       </c>
       <c r="C322" s="1" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="D322" s="1" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="E322" t="s">
         <v>33</v>
@@ -10693,10 +10705,10 @@
         <v>2007</v>
       </c>
       <c r="C323" s="1" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="D323" s="1" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="E323" t="s">
         <v>33</v>
@@ -10720,10 +10732,10 @@
         <v>2008</v>
       </c>
       <c r="C324" s="1" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="D324" s="1" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="E324" t="s">
         <v>33</v>
@@ -10747,10 +10759,10 @@
         <v>2009</v>
       </c>
       <c r="C325" s="1" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="D325" s="1" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="E325" t="s">
         <v>33</v>
@@ -10774,10 +10786,10 @@
         <v>2010</v>
       </c>
       <c r="C326" s="1" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="D326" s="1" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="E326" t="s">
         <v>33</v>
@@ -10801,10 +10813,10 @@
         <v>2011</v>
       </c>
       <c r="C327" s="1" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="D327" s="1" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="E327" t="s">
         <v>33</v>
@@ -10828,10 +10840,10 @@
         <v>2101</v>
       </c>
       <c r="C328" s="1" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="D328" s="1" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="E328" t="s">
         <v>33</v>
@@ -10855,10 +10867,10 @@
         <v>2102</v>
       </c>
       <c r="C329" s="1" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="D329" s="1" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="E329" t="s">
         <v>33</v>
@@ -10882,10 +10894,10 @@
         <v>2103</v>
       </c>
       <c r="C330" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="D330" s="1" t="s">
         <v>350</v>
-      </c>
-      <c r="D330" s="1" t="s">
-        <v>348</v>
       </c>
       <c r="E330" t="s">
         <v>33</v>
@@ -10909,10 +10921,10 @@
         <v>2104</v>
       </c>
       <c r="C331" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="D331" s="1" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="E331" t="s">
         <v>33</v>
@@ -10936,10 +10948,10 @@
         <v>2105</v>
       </c>
       <c r="C332" s="1" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="D332" s="1" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="E332" t="s">
         <v>33</v>
@@ -10963,10 +10975,10 @@
         <v>2106</v>
       </c>
       <c r="C333" s="1" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="D333" s="1" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="E333" t="s">
         <v>33</v>
@@ -10990,10 +11002,10 @@
         <v>2107</v>
       </c>
       <c r="C334" s="1" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="D334" s="1" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="E334" t="s">
         <v>33</v>
@@ -11017,10 +11029,10 @@
         <v>2201</v>
       </c>
       <c r="C335" s="1" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="D335" s="1" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="E335" t="s">
         <v>78</v>
@@ -11047,7 +11059,7 @@
         <v>32</v>
       </c>
       <c r="D336" s="1" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="E336" t="s">
         <v>78</v>
@@ -11071,10 +11083,10 @@
         <v>2203</v>
       </c>
       <c r="C337" s="1" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="D337" s="1" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="E337" t="s">
         <v>78</v>
@@ -11098,10 +11110,10 @@
         <v>2204</v>
       </c>
       <c r="C338" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="D338" s="1" t="s">
         <v>357</v>
-      </c>
-      <c r="D338" s="1" t="s">
-        <v>355</v>
       </c>
       <c r="E338" t="s">
         <v>78</v>
@@ -11125,10 +11137,10 @@
         <v>2205</v>
       </c>
       <c r="C339" s="1" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="D339" s="1" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="E339" t="s">
         <v>78</v>
@@ -11152,10 +11164,10 @@
         <v>2206</v>
       </c>
       <c r="C340" s="1" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="D340" s="1" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="E340" t="s">
         <v>78</v>
@@ -11179,10 +11191,10 @@
         <v>2207</v>
       </c>
       <c r="C341" s="1" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="D341" s="1" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="E341" t="s">
         <v>78</v>
@@ -11206,10 +11218,10 @@
         <v>2208</v>
       </c>
       <c r="C342" s="1" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="D342" s="1" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="E342" t="s">
         <v>78</v>
@@ -11233,10 +11245,10 @@
         <v>2209</v>
       </c>
       <c r="C343" s="1" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="D343" s="1" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="E343" t="s">
         <v>78</v>
@@ -11260,10 +11272,10 @@
         <v>2210</v>
       </c>
       <c r="C344" s="1" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="D344" s="1" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="E344" t="s">
         <v>78</v>
@@ -11287,10 +11299,10 @@
         <v>2211</v>
       </c>
       <c r="C345" s="1" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="D345" s="1" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="E345" t="s">
         <v>78</v>
@@ -11314,10 +11326,10 @@
         <v>2212</v>
       </c>
       <c r="C346" s="1" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="D346" s="1" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="E346" t="s">
         <v>78</v>
@@ -11341,10 +11353,10 @@
         <v>2213</v>
       </c>
       <c r="C347" s="1" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="D347" s="1" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="E347" t="s">
         <v>78</v>
@@ -11368,10 +11380,10 @@
         <v>2214</v>
       </c>
       <c r="C348" s="1" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="D348" s="1" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="E348" t="s">
         <v>78</v>
@@ -11395,10 +11407,10 @@
         <v>2215</v>
       </c>
       <c r="C349" s="1" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="D349" s="1" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="E349" t="s">
         <v>78</v>
@@ -11422,10 +11434,10 @@
         <v>2216</v>
       </c>
       <c r="C350" s="1" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="D350" s="1" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="E350" t="s">
         <v>78</v>
@@ -11449,10 +11461,10 @@
         <v>2217</v>
       </c>
       <c r="C351" s="1" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="D351" s="1" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="E351" t="s">
         <v>78</v>

</xml_diff>